<commit_message>
Correct fragment-like set(molecule with logP). Vendor based list updated for both sets.
</commit_message>
<xml_diff>
--- a/compound_selection/zinc15_eMolecules_intersection_set/20170811_zinc15_eMolecules_subset_group_by_vendor/df_frag_final_supplier_oe_printable.xlsx
+++ b/compound_selection/zinc15_eMolecules_intersection_set/20170811_zinc15_eMolecules_subset_group_by_vendor/df_frag_final_supplier_oe_printable.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26004"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="23620" windowHeight="13940"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="239">
   <si>
     <t>df_frag_final_supplier_oe.csv</t>
   </si>
@@ -54,12 +54,18 @@
     <t>N_UV_chrom</t>
   </si>
   <si>
+    <t>Selection</t>
+  </si>
+  <si>
     <t>Bin index</t>
   </si>
   <si>
     <t>Priority</t>
   </si>
   <si>
+    <t>Final list</t>
+  </si>
+  <si>
     <t>Supplier Name</t>
   </si>
   <si>
@@ -96,12 +102,18 @@
     <t>27</t>
   </si>
   <si>
+    <t>picked</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
+    <t>True</t>
+  </si>
+  <si>
     <t>ChemDiv</t>
   </si>
   <si>
@@ -189,6 +201,9 @@
     <t>[5.564]</t>
   </si>
   <si>
+    <t>269.72900000000004</t>
+  </si>
+  <si>
     <t>415.5</t>
   </si>
   <si>
@@ -594,6 +609,9 @@
     <t>[4.294]</t>
   </si>
   <si>
+    <t>331.36800000000005</t>
+  </si>
+  <si>
     <t>159.0</t>
   </si>
   <si>
@@ -682,6 +700,9 @@
   </si>
   <si>
     <t>[8.052]</t>
+  </si>
+  <si>
+    <t>323.7270000000001</t>
   </si>
   <si>
     <t>125.0</t>
@@ -721,7 +742,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,10 +751,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -790,33 +840,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,7 +895,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>165182</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -878,7 +933,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>63582</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -916,7 +971,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>139782</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -954,7 +1009,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>63582</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -992,7 +1047,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>330282</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1029,8 +1084,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1068,7 +1123,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>25482</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1106,7 +1161,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>139782</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1144,7 +1199,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>12782</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1220,7 +1275,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>38182</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1258,7 +1313,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>279482</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1296,7 +1351,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>279482</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1333,8 +1388,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1372,7 +1427,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>50882</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1409,8 +1464,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1447,8 +1502,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1486,7 +1541,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>50882</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1523,8 +1578,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1562,7 +1617,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>101682</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1599,8 +1654,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1638,7 +1693,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>101682</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1675,8 +1730,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1713,8 +1768,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1587582</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1752,7 +1807,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1587582</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>76282</xdr:rowOff>
+      <xdr:rowOff>127082</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2067,1271 +2122,1472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="37.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="8" customWidth="1"/>
-    <col min="9" max="9" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.1640625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="8"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="23">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="23">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="Q2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="112" customHeight="1">
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5">
+    <row r="3" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8">
         <v>0.71999996900558405</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="K3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="L3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="N3" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="O3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" s="6" customFormat="1" ht="120" customHeight="1">
+    <row r="4" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3.2689995765686</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3.2689995765686</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="P4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3.79499983787536</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="9">
+        <v>3.5230002403259202</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3.6050002574920601</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2.90700030326843</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2.9229996204376198</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2.8030002117156898</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="6" t="s">
+      <c r="D11" s="8">
+        <v>3.1389999389648402</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="L11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2.3329999446868799</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2.21900033950805</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2.7179999351501398</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="8">
+        <v>4.2330002784728897</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="9">
+        <v>2.5950002670288002</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="8">
+        <v>4.1289997100829998</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1.49900019168853</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="8">
+        <v>3.8990001678466801</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="9">
+        <v>2.4399998188018799</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="6" t="s">
+      <c r="J20" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="R20" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2.9270000457763601</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="9">
+        <v>3.0820000171661301</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D23" s="8">
+        <v>3.3059999942779501</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="M23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>209</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="114" customHeight="1">
-      <c r="B5" s="4" t="s">
+    <row r="24" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D24" s="9">
+        <v>2.1920003890991202</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3.79499983787536</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="4" t="s">
+      <c r="J24" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D25" s="8">
+        <v>3.7479996681213299</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>53</v>
       </c>
+      <c r="M25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" ht="120" customHeight="1">
-      <c r="B6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="7">
-        <v>3.5230002403259202</v>
-      </c>
-      <c r="E6" s="10">
-        <v>269.72899999999998</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>59</v>
+    <row r="26" spans="1:18" s="3" customFormat="1" ht="115" customHeight="1">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="9">
+        <v>3.9079997539520201</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="99" customHeight="1">
-      <c r="B7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="5">
-        <v>3.6050002574920601</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" s="6" customFormat="1" ht="128" customHeight="1">
-      <c r="B8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="7">
-        <v>2.90700030326843</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" ht="123" customHeight="1">
-      <c r="B9" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2.9229996204376198</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="6" customFormat="1" ht="114" customHeight="1">
-      <c r="B10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="7">
-        <v>2.8030002117156898</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" ht="124" customHeight="1">
-      <c r="B11" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="5">
-        <v>3.1389999389648402</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="6" customFormat="1" ht="115" customHeight="1">
-      <c r="B12" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="7">
-        <v>2.3329999446868799</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="4" customFormat="1" ht="122" customHeight="1">
-      <c r="B13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="5">
-        <v>2.21900033950805</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="6" customFormat="1" ht="103" customHeight="1">
-      <c r="B14" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="7">
-        <v>2.7179999351501398</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="4" customFormat="1" ht="103" customHeight="1">
-      <c r="B15" s="4" t="s">
+    <row r="27" spans="1:18" s="2" customFormat="1" ht="115" customHeight="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D27" s="8">
+        <v>4.0799999237060502</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="J27" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D15" s="5">
-        <v>4.2330002784728897</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="6" customFormat="1" ht="128" customHeight="1">
-      <c r="B16" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="7">
-        <v>2.5950002670288002</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" s="4" customFormat="1" ht="121" customHeight="1">
-      <c r="B17" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4.1289997100829998</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" s="6" customFormat="1" ht="129" customHeight="1">
-      <c r="B18" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="K27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="7">
-        <v>1.49900019168853</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" s="4" customFormat="1" ht="127" customHeight="1">
-      <c r="B19" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="5">
-        <v>3.8990001678466801</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="N19" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="O19" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" s="6" customFormat="1" ht="121" customHeight="1">
-      <c r="B20" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D20" s="7">
-        <v>2.4399998188018799</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="P20" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" s="4" customFormat="1" ht="126" customHeight="1">
-      <c r="B21" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="M27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="5">
-        <v>2.9270000457763601</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" s="6" customFormat="1" ht="117" customHeight="1">
-      <c r="B22" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3.0820000171661301</v>
-      </c>
-      <c r="E22" s="10">
-        <v>331.36799999999999</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P22" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" s="4" customFormat="1" ht="128" customHeight="1">
-      <c r="B23" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D23" s="5">
-        <v>3.3059999942779501</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="O23" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" s="6" customFormat="1" ht="117" customHeight="1">
-      <c r="B24" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D24" s="7">
-        <v>2.1920003890991202</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="O24" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" s="4" customFormat="1" ht="135" customHeight="1">
-      <c r="B25" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" s="5">
-        <v>3.7479996681213299</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="N25" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" s="6" customFormat="1" ht="126" customHeight="1">
-      <c r="B26" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D26" s="7">
-        <v>3.9079997539520201</v>
-      </c>
-      <c r="E26" s="10">
-        <v>323.72699999999998</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="O26" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" s="4" customFormat="1" ht="119" customHeight="1">
-      <c r="B27" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D27" s="5">
-        <v>4.0799999237060502</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="N27" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="O27" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="P27" s="4" t="s">
-        <v>231</v>
+      <c r="P27" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="R27" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="30" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="18" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>